<commit_message>
excel to string array dynamic
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Company\Payment Networks2\selenium_workspace\OrangeHRMAutomation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Balaji</t>
-  </si>
-  <si>
-    <t>Peter</t>
   </si>
   <si>
     <t>Invalid credentials</t>
@@ -386,7 +383,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,18 +401,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
+      <c r="A2">
+        <v>1122</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -426,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validcredential test connected with excel
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Expected Error</t>
+  </si>
+  <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>john</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +429,28 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>